<commit_message>
uploading data for recreating oecd chart post
</commit_message>
<xml_diff>
--- a/content/post/2021-26-03-recreating-oecd-chart/data.xlsx
+++ b/content/post/2021-26-03-recreating-oecd-chart/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnoel\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\joliennoels\content\post\2021-26-03-recreating-oecd-chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85033F5-CAE0-434A-B7F3-2CEF70920334}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2076C6F-33D0-4E11-92FD-F0A283202C53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3448,12 +3448,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties">
-  <LongProp xmlns="" name="OECDProjectMembers"><![CDATA[107;#CARCILLO Stéphane, ELS/JAI;#146;#BASSANINI Andrea, ELS/JAI;#122;#SWAIM Paul, ELS/MSU;#113;#PARENT Gwenn, ELS/MSU;#1192;#BEYELER Brigitte, ELS/JAI;#167;#PUYMOYEN Agnès, ELS/JAI;#158;#CIMPER Sylvie, ELS/SAE;#105;#HIJZEN Alexander, ELS/JAI;#202;#CORRY Natalie, ELS/JAI;#132;#GARNERO Andrea, ELS/JAI;#381;#CAZES Sandrine, ELS/JAI;#968;#DENK Oliver, ELS/JAI;#98;#IMMERVOLL Herwig, ELS/JAI;#220;#BLUMIN Dana, ELS/SAE;#741;#MACDONALD Duncan, ELS/SAE;#147;#MARIANNA Pascal, ELS/SAE;#201;#MARTIN Sebastien, ELS/JAI;#884;#GEORGIEFF Alexandre, ELS/JAI;#150;#FERNANDEZ Rodrigo, ELS/JAI;#179;#PACIFICO Daniele, ELS/JAI;#155;#FALCO Paolo, ELS/SAE]]></LongProp>
-</LongProperties>
+<?mso-contentType ?>
+<CtFieldPriority xmlns="http://www.oecd.org/eshare/projectsentre/CtFieldPriority/" xmlns:i="http://www.w3.org/2001/XMLSchema-instance">
+  <PriorityFields xmlns:a="http://schemas.microsoft.com/2003/10/Serialization/Arrays">
+    <a:string>Title</a:string>
+    <a:string>OECDCountry</a:string>
+    <a:string>OECDTopic</a:string>
+    <a:string>OECDKeywords</a:string>
+  </PriorityFields>
+</CtFieldPriority>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>OECDListFormCollapsible</Display>
+  <Edit>OECDListFormCollapsible</Edit>
+  <New>OECDListFormCollapsible</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Working Document" ma:contentTypeID="0x0101008B4DD370EC31429186F3AD49F0D3098F00D44DBCB9EB4F45278CB5C9765BE5299500A4858B360C6A491AA753F8BCA47AA9100033AB0B45A31F2B489F9B80276A6B0922" ma:contentTypeVersion="70" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="d5d78593aaa09c188e19b92e9fb57eb0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="54c4cd27-f286-408f-9ce0-33c1e0f3ab39" xmlns:ns3="c5805097-db0a-42f9-a837-be9035f1f571" xmlns:ns4="ca82dde9-3436-4d3d-bddd-d31447390034" xmlns:ns5="22a5b7d0-1699-458f-b8e2-4d8247229549" xmlns:ns6="c9f238dd-bb73-4aef-a7a5-d644ad823e52" xmlns:ns7="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e63d84065b627076c456af879a2eda7c" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="" ns7:_="">
     <xsd:import namespace="54c4cd27-f286-408f-9ce0-33c1e0f3ab39"/>
@@ -3876,28 +3891,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>OECDListFormCollapsible</Display>
-  <Edit>OECDListFormCollapsible</Edit>
-  <New>OECDListFormCollapsible</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<CtFieldPriority xmlns="http://www.oecd.org/eshare/projectsentre/CtFieldPriority/" xmlns:i="http://www.w3.org/2001/XMLSchema-instance">
-  <PriorityFields xmlns:a="http://schemas.microsoft.com/2003/10/Serialization/Arrays">
-    <a:string>Title</a:string>
-    <a:string>OECDCountry</a:string>
-    <a:string>OECDTopic</a:string>
-    <a:string>OECDKeywords</a:string>
-  </PriorityFields>
-</CtFieldPriority>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties">
+  <LongProp xmlns="" name="OECDProjectMembers"><![CDATA[107;#CARCILLO Stéphane, ELS/JAI;#146;#BASSANINI Andrea, ELS/JAI;#122;#SWAIM Paul, ELS/MSU;#113;#PARENT Gwenn, ELS/MSU;#1192;#BEYELER Brigitte, ELS/JAI;#167;#PUYMOYEN Agnès, ELS/JAI;#158;#CIMPER Sylvie, ELS/SAE;#105;#HIJZEN Alexander, ELS/JAI;#202;#CORRY Natalie, ELS/JAI;#132;#GARNERO Andrea, ELS/JAI;#381;#CAZES Sandrine, ELS/JAI;#968;#DENK Oliver, ELS/JAI;#98;#IMMERVOLL Herwig, ELS/JAI;#220;#BLUMIN Dana, ELS/SAE;#741;#MACDONALD Duncan, ELS/SAE;#147;#MARIANNA Pascal, ELS/SAE;#201;#MARTIN Sebastien, ELS/JAI;#884;#GEORGIEFF Alexandre, ELS/JAI;#150;#FERNANDEZ Rodrigo, ELS/JAI;#179;#PACIFICO Daniele, ELS/JAI;#155;#FALCO Paolo, ELS/SAE]]></LongProp>
+</LongProperties>
 </file>
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="27ec883c-a62c-444f-a935-fcddb579e39d" ContentTypeId="0x0101008B4DD370EC31429186F3AD49F0D3098F00D44DBCB9EB4F45278CB5C9765BE52995" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <eShareHorizProjTaxHTField0 xmlns="c5805097-db0a-42f9-a837-be9035f1f571" xsi:nil="true"/>
@@ -4082,21 +4087,24 @@
 </p:properties>
 </file>
 
-<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="27ec883c-a62c-444f-a935-fcddb579e39d" ContentTypeId="0x0101008B4DD370EC31429186F3AD49F0D3098F00D44DBCB9EB4F45278CB5C9765BE52995" PreviousValue="false"/>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51D5AD65-ED9E-4BB8-836F-D4862FEAD6C4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9166C2F6-8F09-4B51-932B-41A2E0FE54EC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-    <ds:schemaRef ds:uri=""/>
+    <ds:schemaRef ds:uri="http://www.oecd.org/eshare/projectsentre/CtFieldPriority/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/2003/10/Serialization/Arrays"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77556ACC-CB52-4EA0-BDFC-D40F47EE5EB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA986C8E-7458-48DC-83F6-6A21E6AD2768}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4119,24 +4127,24 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77556ACC-CB52-4EA0-BDFC-D40F47EE5EB8}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51D5AD65-ED9E-4BB8-836F-D4862FEAD6C4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9166C2F6-8F09-4B51-932B-41A2E0FE54EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.oecd.org/eshare/projectsentre/CtFieldPriority/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/2003/10/Serialization/Arrays"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri=""/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AED980B-5A32-4AA4-AD4E-E0CB4DF3F912}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{770F42DD-6869-40DC-9685-248206AE57E8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4149,12 +4157,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AED980B-5A32-4AA4-AD4E-E0CB4DF3F912}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>